<commit_message>
IN and LIKE Operators
</commit_message>
<xml_diff>
--- a/me/6.Salesforce-Object-Query-Language.xlsx
+++ b/me/6.Salesforce-Object-Query-Language.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\salesforce\me\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB7896C3-E33E-4F3C-AB30-BC0274DE34D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1A4E164-4BE8-4761-A254-03B62B32BF2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Salesforce Objects and Fields" sheetId="1" r:id="rId1"/>
     <sheet name="Understand SOQL" sheetId="2" r:id="rId2"/>
     <sheet name="WHERE ClauseAND and OR Operator" sheetId="3" r:id="rId3"/>
+    <sheet name="IN and LIKE Operators" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="36">
   <si>
     <t>Accounts table</t>
   </si>
@@ -108,6 +109,77 @@
   </si>
   <si>
     <t>SELECT Name, Status, LeadSource, Company, Email FROM Lead WHERE (Status='Closed - Converted' OR Status='Closed - Not Converted') AND LeadSource='Web'</t>
+  </si>
+  <si>
+    <t>3.soql-in-and-like-operator</t>
+  </si>
+  <si>
+    <t>salesforce\6.Salesforce-Object-Query-Language\3.soql-in-and-like-operator\queries.txt</t>
+  </si>
+  <si>
+    <t>// IN Operator</t>
+  </si>
+  <si>
+    <t>SELECT Name, Status, LeadSource, Company, Email FROM Lead WHERE Status IN ('Closed - Converted', 'Closed - Not Converted') AND LeadSource='Web'</t>
+  </si>
+  <si>
+    <t>// LIKE Operator</t>
+  </si>
+  <si>
+    <t>SELECT Name, Status, LeadSource, Company, Email FROM Lead WHERE Status LIKE 'Closed%' AND LeadSource='Web'</t>
+  </si>
+  <si>
+    <t>=</t>
+  </si>
+  <si>
+    <r>
+      <t>SELECT Name, Status, LeadSource, Company, Email FROM Lead WHERE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Status IN ('Closed - Converted', 'Closed - Not Converted')</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> AND LeadSource='Web'</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">SELECT Name, Status, LeadSource, Company, Email FROM Lead WHERE </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">(Status='Closed - Converted' OR Status='Closed - Not Converted') </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>AND LeadSource='Web'</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -2965,6 +3037,376 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>120422</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{69C500B7-409B-CFED-38C4-0117C70BA20B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="685800" y="5191125"/>
+          <a:ext cx="11049000" cy="5597297"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>333375</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>466725</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="5" name="Straight Arrow Connector 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E999206F-987A-31F5-5A5C-D50E8B0FC59E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="3381375" y="5086350"/>
+          <a:ext cx="2571750" cy="2000250"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>514350</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="7" name="Straight Arrow Connector 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{405977CC-AEF0-F4E6-78C0-301ABEA59F25}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="3790950" y="5067300"/>
+          <a:ext cx="3429000" cy="1838325"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="9" name="Straight Arrow Connector 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D4CB9352-3B98-2F8C-AD3B-DBE4044E8FEA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="5715000" y="5105400"/>
+          <a:ext cx="3543300" cy="1790700"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>89</xdr:row>
+      <xdr:rowOff>65209</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="12" name="Picture 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{43596015-43E0-073F-2420-5DD93EE13268}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="695325" y="11458575"/>
+          <a:ext cx="10953750" cy="5561134"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>70</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>447675</xdr:colOff>
+      <xdr:row>78</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="14" name="Straight Arrow Connector 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{29680E14-ED74-631F-094E-0F20DB118772}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="3190875" y="13420725"/>
+          <a:ext cx="2133600" cy="1609725"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>504825</xdr:colOff>
+      <xdr:row>70</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>78</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="16" name="Straight Arrow Connector 15">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E7A4AA05-F102-CDDC-52F5-FA314DB98496}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="5381625" y="13439775"/>
+          <a:ext cx="1333500" cy="1600200"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -6780,8 +7222,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C024AD3B-EA8D-492C-A299-F36217497030}">
   <dimension ref="A3:T90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="A58" sqref="A58"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6833,28 +7275,22 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B9" s="4"/>
-      <c r="C9" s="13" t="s">
+      <c r="C9" t="s">
         <v>12</v>
       </c>
-      <c r="D9" s="13"/>
-      <c r="E9" s="13"/>
       <c r="F9" s="11"/>
       <c r="H9" s="5"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B10" s="4"/>
-      <c r="C10" s="13"/>
-      <c r="D10" s="13" t="s">
+      <c r="D10" t="s">
         <v>15</v>
       </c>
-      <c r="E10" s="13"/>
       <c r="H10" s="5"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B11" s="4"/>
-      <c r="C11" s="13"/>
-      <c r="D11" s="13"/>
-      <c r="E11" s="13" t="s">
+      <c r="E11" t="s">
         <v>16</v>
       </c>
       <c r="H11" s="5"/>
@@ -6927,58 +7363,16 @@
       <c r="B19" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="C19" s="14"/>
-      <c r="D19" s="14"/>
-      <c r="E19" s="14"/>
-      <c r="F19" s="14"/>
-      <c r="G19" s="14"/>
-      <c r="H19" s="14"/>
-      <c r="I19" s="14"/>
-      <c r="J19" s="14"/>
-      <c r="K19" s="14"/>
-      <c r="L19" s="14"/>
-      <c r="M19" s="14"/>
-      <c r="N19" s="14"/>
-      <c r="O19" s="14"/>
-      <c r="P19" s="14"/>
       <c r="Q19" s="5"/>
     </row>
     <row r="20" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B20" s="4"/>
-      <c r="C20" s="14"/>
-      <c r="D20" s="14"/>
-      <c r="E20" s="14"/>
-      <c r="F20" s="14"/>
-      <c r="G20" s="14"/>
-      <c r="H20" s="14"/>
-      <c r="I20" s="14"/>
-      <c r="J20" s="14"/>
-      <c r="K20" s="14"/>
-      <c r="L20" s="14"/>
-      <c r="M20" s="14"/>
-      <c r="N20" s="14"/>
-      <c r="O20" s="14"/>
-      <c r="P20" s="14"/>
       <c r="Q20" s="5"/>
     </row>
     <row r="21" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B21" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C21" s="14"/>
-      <c r="D21" s="14"/>
-      <c r="E21" s="14"/>
-      <c r="F21" s="14"/>
-      <c r="G21" s="14"/>
-      <c r="H21" s="14"/>
-      <c r="I21" s="14"/>
-      <c r="J21" s="14"/>
-      <c r="K21" s="14"/>
-      <c r="L21" s="14"/>
-      <c r="M21" s="14"/>
-      <c r="N21" s="14"/>
-      <c r="O21" s="14"/>
-      <c r="P21" s="14"/>
       <c r="Q21" s="5"/>
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.25">
@@ -7026,632 +7420,122 @@
     </row>
     <row r="26" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B26" s="4"/>
-      <c r="C26" s="14"/>
-      <c r="D26" s="14"/>
-      <c r="E26" s="14"/>
-      <c r="F26" s="14"/>
-      <c r="G26" s="14"/>
-      <c r="H26" s="14"/>
-      <c r="I26" s="14"/>
-      <c r="J26" s="14"/>
-      <c r="K26" s="14"/>
-      <c r="L26" s="14"/>
-      <c r="M26" s="14"/>
-      <c r="N26" s="14"/>
-      <c r="O26" s="14"/>
-      <c r="P26" s="14"/>
-      <c r="Q26" s="14"/>
-      <c r="R26" s="14"/>
-      <c r="S26" s="14"/>
       <c r="T26" s="5"/>
     </row>
     <row r="27" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B27" s="4"/>
-      <c r="C27" s="14"/>
-      <c r="D27" s="14"/>
-      <c r="E27" s="14"/>
-      <c r="F27" s="14"/>
-      <c r="G27" s="14"/>
-      <c r="H27" s="14"/>
-      <c r="I27" s="14"/>
-      <c r="J27" s="14"/>
-      <c r="K27" s="14"/>
-      <c r="L27" s="14"/>
-      <c r="M27" s="14"/>
-      <c r="N27" s="14"/>
-      <c r="O27" s="14"/>
-      <c r="P27" s="14"/>
-      <c r="Q27" s="14"/>
-      <c r="R27" s="14"/>
-      <c r="S27" s="14"/>
       <c r="T27" s="5"/>
     </row>
     <row r="28" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B28" s="4"/>
-      <c r="C28" s="14"/>
-      <c r="D28" s="14"/>
-      <c r="E28" s="14"/>
-      <c r="F28" s="14"/>
-      <c r="G28" s="14"/>
-      <c r="H28" s="14"/>
-      <c r="I28" s="14"/>
-      <c r="J28" s="14"/>
-      <c r="K28" s="14"/>
-      <c r="L28" s="14"/>
-      <c r="M28" s="14"/>
-      <c r="N28" s="14"/>
-      <c r="O28" s="14"/>
-      <c r="P28" s="14"/>
-      <c r="Q28" s="14"/>
-      <c r="R28" s="14"/>
-      <c r="S28" s="14"/>
       <c r="T28" s="5"/>
     </row>
     <row r="29" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B29" s="4"/>
-      <c r="C29" s="14"/>
-      <c r="D29" s="14"/>
-      <c r="E29" s="14"/>
-      <c r="F29" s="14"/>
-      <c r="G29" s="14"/>
-      <c r="H29" s="14"/>
-      <c r="I29" s="14"/>
-      <c r="J29" s="14"/>
-      <c r="K29" s="14"/>
-      <c r="L29" s="14"/>
-      <c r="M29" s="14"/>
-      <c r="N29" s="14"/>
-      <c r="O29" s="14"/>
-      <c r="P29" s="14"/>
-      <c r="Q29" s="14"/>
-      <c r="R29" s="14"/>
-      <c r="S29" s="14"/>
       <c r="T29" s="5"/>
     </row>
     <row r="30" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B30" s="4"/>
-      <c r="C30" s="14"/>
-      <c r="D30" s="14"/>
-      <c r="E30" s="14"/>
-      <c r="F30" s="14"/>
-      <c r="G30" s="14"/>
-      <c r="H30" s="14"/>
-      <c r="I30" s="14"/>
-      <c r="J30" s="14"/>
-      <c r="K30" s="14"/>
-      <c r="L30" s="14"/>
-      <c r="M30" s="14"/>
-      <c r="N30" s="14"/>
-      <c r="O30" s="14"/>
-      <c r="P30" s="14"/>
-      <c r="Q30" s="14"/>
-      <c r="R30" s="14"/>
-      <c r="S30" s="14"/>
       <c r="T30" s="5"/>
     </row>
     <row r="31" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B31" s="4"/>
-      <c r="C31" s="14"/>
-      <c r="D31" s="14"/>
-      <c r="E31" s="14"/>
-      <c r="F31" s="14"/>
-      <c r="G31" s="14"/>
-      <c r="H31" s="14"/>
-      <c r="I31" s="14"/>
-      <c r="J31" s="14"/>
-      <c r="K31" s="14"/>
-      <c r="L31" s="14"/>
-      <c r="M31" s="14"/>
-      <c r="N31" s="14"/>
-      <c r="O31" s="14"/>
-      <c r="P31" s="14"/>
-      <c r="Q31" s="14"/>
-      <c r="R31" s="14"/>
-      <c r="S31" s="14"/>
       <c r="T31" s="5"/>
     </row>
     <row r="32" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B32" s="4"/>
-      <c r="C32" s="14"/>
-      <c r="D32" s="14"/>
-      <c r="E32" s="14"/>
-      <c r="F32" s="14"/>
-      <c r="G32" s="14"/>
-      <c r="H32" s="14"/>
-      <c r="I32" s="14"/>
-      <c r="J32" s="14"/>
-      <c r="K32" s="14"/>
-      <c r="L32" s="14"/>
-      <c r="M32" s="14"/>
-      <c r="N32" s="14"/>
-      <c r="O32" s="14"/>
-      <c r="P32" s="14"/>
-      <c r="Q32" s="14"/>
-      <c r="R32" s="14"/>
-      <c r="S32" s="14"/>
       <c r="T32" s="5"/>
     </row>
     <row r="33" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B33" s="4"/>
-      <c r="C33" s="14"/>
-      <c r="D33" s="14"/>
-      <c r="E33" s="14"/>
-      <c r="F33" s="14"/>
-      <c r="G33" s="14"/>
-      <c r="H33" s="14"/>
-      <c r="I33" s="14"/>
-      <c r="J33" s="14"/>
-      <c r="K33" s="14"/>
-      <c r="L33" s="14"/>
-      <c r="M33" s="14"/>
-      <c r="N33" s="14"/>
-      <c r="O33" s="14"/>
-      <c r="P33" s="14"/>
-      <c r="Q33" s="14"/>
-      <c r="R33" s="14"/>
-      <c r="S33" s="14"/>
       <c r="T33" s="5"/>
     </row>
     <row r="34" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B34" s="4"/>
-      <c r="C34" s="14"/>
-      <c r="D34" s="14"/>
-      <c r="E34" s="14"/>
-      <c r="F34" s="14"/>
-      <c r="G34" s="14"/>
-      <c r="H34" s="14"/>
-      <c r="I34" s="14"/>
-      <c r="J34" s="14"/>
-      <c r="K34" s="14"/>
-      <c r="L34" s="14"/>
-      <c r="M34" s="14"/>
-      <c r="N34" s="14"/>
-      <c r="O34" s="14"/>
-      <c r="P34" s="14"/>
-      <c r="Q34" s="14"/>
-      <c r="R34" s="14"/>
-      <c r="S34" s="14"/>
       <c r="T34" s="5"/>
     </row>
     <row r="35" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B35" s="4"/>
-      <c r="C35" s="14"/>
-      <c r="D35" s="14"/>
-      <c r="E35" s="14"/>
-      <c r="F35" s="14"/>
-      <c r="G35" s="14"/>
-      <c r="H35" s="14"/>
-      <c r="I35" s="14"/>
-      <c r="J35" s="14"/>
-      <c r="K35" s="14"/>
-      <c r="L35" s="14"/>
-      <c r="M35" s="14"/>
-      <c r="N35" s="14"/>
-      <c r="O35" s="14"/>
-      <c r="P35" s="14"/>
-      <c r="Q35" s="14"/>
-      <c r="R35" s="14"/>
-      <c r="S35" s="14"/>
       <c r="T35" s="5"/>
     </row>
     <row r="36" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B36" s="4"/>
-      <c r="C36" s="14"/>
-      <c r="D36" s="14"/>
-      <c r="E36" s="14"/>
-      <c r="F36" s="14"/>
-      <c r="G36" s="14"/>
-      <c r="H36" s="14"/>
-      <c r="I36" s="14"/>
-      <c r="J36" s="14"/>
-      <c r="K36" s="14"/>
-      <c r="L36" s="14"/>
-      <c r="M36" s="14"/>
-      <c r="N36" s="14"/>
-      <c r="O36" s="14"/>
-      <c r="P36" s="14"/>
-      <c r="Q36" s="14"/>
-      <c r="R36" s="14"/>
-      <c r="S36" s="14"/>
       <c r="T36" s="5"/>
     </row>
     <row r="37" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B37" s="4"/>
-      <c r="C37" s="14"/>
-      <c r="D37" s="14"/>
-      <c r="E37" s="14"/>
-      <c r="F37" s="14"/>
-      <c r="G37" s="14"/>
-      <c r="H37" s="14"/>
-      <c r="I37" s="14"/>
-      <c r="J37" s="14"/>
-      <c r="K37" s="14"/>
-      <c r="L37" s="14"/>
-      <c r="M37" s="14"/>
-      <c r="N37" s="14"/>
-      <c r="O37" s="14"/>
-      <c r="P37" s="14"/>
-      <c r="Q37" s="14"/>
-      <c r="R37" s="14"/>
-      <c r="S37" s="14"/>
       <c r="T37" s="5"/>
     </row>
     <row r="38" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B38" s="4"/>
-      <c r="C38" s="14"/>
-      <c r="D38" s="14"/>
-      <c r="E38" s="14"/>
-      <c r="F38" s="14"/>
-      <c r="G38" s="14"/>
-      <c r="H38" s="14"/>
-      <c r="I38" s="14"/>
-      <c r="J38" s="14"/>
-      <c r="K38" s="14"/>
-      <c r="L38" s="14"/>
-      <c r="M38" s="14"/>
-      <c r="N38" s="14"/>
-      <c r="O38" s="14"/>
-      <c r="P38" s="14"/>
-      <c r="Q38" s="14"/>
-      <c r="R38" s="14"/>
-      <c r="S38" s="14"/>
       <c r="T38" s="5"/>
     </row>
     <row r="39" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B39" s="4"/>
-      <c r="C39" s="14"/>
-      <c r="D39" s="14"/>
-      <c r="E39" s="14"/>
-      <c r="F39" s="14"/>
-      <c r="G39" s="14"/>
-      <c r="H39" s="14"/>
-      <c r="I39" s="14"/>
-      <c r="J39" s="14"/>
-      <c r="K39" s="14"/>
-      <c r="L39" s="14"/>
-      <c r="M39" s="14"/>
-      <c r="N39" s="14"/>
-      <c r="O39" s="14"/>
-      <c r="P39" s="14"/>
-      <c r="Q39" s="14"/>
-      <c r="R39" s="14"/>
-      <c r="S39" s="14"/>
       <c r="T39" s="5"/>
     </row>
     <row r="40" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B40" s="4"/>
-      <c r="C40" s="14"/>
-      <c r="D40" s="14"/>
-      <c r="E40" s="14"/>
-      <c r="F40" s="14"/>
-      <c r="G40" s="14"/>
-      <c r="H40" s="14"/>
-      <c r="I40" s="14"/>
-      <c r="J40" s="14"/>
-      <c r="K40" s="14"/>
-      <c r="L40" s="14"/>
-      <c r="M40" s="14"/>
-      <c r="N40" s="14"/>
-      <c r="O40" s="14"/>
-      <c r="P40" s="14"/>
-      <c r="Q40" s="14"/>
-      <c r="R40" s="14"/>
-      <c r="S40" s="14"/>
       <c r="T40" s="5"/>
     </row>
     <row r="41" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B41" s="4"/>
-      <c r="C41" s="14"/>
-      <c r="D41" s="14"/>
-      <c r="E41" s="14"/>
-      <c r="F41" s="14"/>
-      <c r="G41" s="14"/>
-      <c r="H41" s="14"/>
-      <c r="I41" s="14"/>
-      <c r="J41" s="14"/>
-      <c r="K41" s="14"/>
-      <c r="L41" s="14"/>
-      <c r="M41" s="14"/>
-      <c r="N41" s="14"/>
-      <c r="O41" s="14"/>
-      <c r="P41" s="14"/>
-      <c r="Q41" s="14"/>
-      <c r="R41" s="14"/>
-      <c r="S41" s="14"/>
       <c r="T41" s="5"/>
     </row>
     <row r="42" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B42" s="4"/>
-      <c r="C42" s="14"/>
-      <c r="D42" s="14"/>
-      <c r="E42" s="14"/>
-      <c r="F42" s="14"/>
-      <c r="G42" s="14"/>
-      <c r="H42" s="14"/>
-      <c r="I42" s="14"/>
-      <c r="J42" s="14"/>
-      <c r="K42" s="14"/>
-      <c r="L42" s="14"/>
-      <c r="M42" s="14"/>
-      <c r="N42" s="14"/>
-      <c r="O42" s="14"/>
-      <c r="P42" s="14"/>
-      <c r="Q42" s="14"/>
-      <c r="R42" s="14"/>
-      <c r="S42" s="14"/>
       <c r="T42" s="5"/>
     </row>
     <row r="43" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B43" s="4"/>
-      <c r="C43" s="14"/>
-      <c r="D43" s="14"/>
-      <c r="E43" s="14"/>
-      <c r="F43" s="14"/>
-      <c r="G43" s="14"/>
-      <c r="H43" s="14"/>
-      <c r="I43" s="14"/>
-      <c r="J43" s="14"/>
-      <c r="K43" s="14"/>
-      <c r="L43" s="14"/>
-      <c r="M43" s="14"/>
-      <c r="N43" s="14"/>
-      <c r="O43" s="14"/>
-      <c r="P43" s="14"/>
-      <c r="Q43" s="14"/>
-      <c r="R43" s="14"/>
-      <c r="S43" s="14"/>
       <c r="T43" s="5"/>
     </row>
     <row r="44" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B44" s="4"/>
-      <c r="C44" s="14"/>
-      <c r="D44" s="14"/>
-      <c r="E44" s="14"/>
-      <c r="F44" s="14"/>
-      <c r="G44" s="14"/>
-      <c r="H44" s="14"/>
-      <c r="I44" s="14"/>
-      <c r="J44" s="14"/>
-      <c r="K44" s="14"/>
-      <c r="L44" s="14"/>
-      <c r="M44" s="14"/>
-      <c r="N44" s="14"/>
-      <c r="O44" s="14"/>
-      <c r="P44" s="14"/>
-      <c r="Q44" s="14"/>
-      <c r="R44" s="14"/>
-      <c r="S44" s="14"/>
       <c r="T44" s="5"/>
     </row>
     <row r="45" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B45" s="4"/>
-      <c r="C45" s="14"/>
-      <c r="D45" s="14"/>
-      <c r="E45" s="14"/>
-      <c r="F45" s="14"/>
-      <c r="G45" s="14"/>
-      <c r="H45" s="14"/>
-      <c r="I45" s="14"/>
-      <c r="J45" s="14"/>
-      <c r="K45" s="14"/>
-      <c r="L45" s="14"/>
-      <c r="M45" s="14"/>
-      <c r="N45" s="14"/>
-      <c r="O45" s="14"/>
-      <c r="P45" s="14"/>
-      <c r="Q45" s="14"/>
-      <c r="R45" s="14"/>
-      <c r="S45" s="14"/>
       <c r="T45" s="5"/>
     </row>
     <row r="46" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B46" s="4"/>
-      <c r="C46" s="14"/>
-      <c r="D46" s="14"/>
-      <c r="E46" s="14"/>
-      <c r="F46" s="14"/>
-      <c r="G46" s="14"/>
-      <c r="H46" s="14"/>
-      <c r="I46" s="14"/>
-      <c r="J46" s="14"/>
-      <c r="K46" s="14"/>
-      <c r="L46" s="14"/>
-      <c r="M46" s="14"/>
-      <c r="N46" s="14"/>
-      <c r="O46" s="14"/>
-      <c r="P46" s="14"/>
-      <c r="Q46" s="14"/>
-      <c r="R46" s="14"/>
-      <c r="S46" s="14"/>
       <c r="T46" s="5"/>
     </row>
     <row r="47" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B47" s="4"/>
-      <c r="C47" s="14"/>
-      <c r="D47" s="14"/>
-      <c r="E47" s="14"/>
-      <c r="F47" s="14"/>
-      <c r="G47" s="14"/>
-      <c r="H47" s="14"/>
-      <c r="I47" s="14"/>
-      <c r="J47" s="14"/>
-      <c r="K47" s="14"/>
-      <c r="L47" s="14"/>
-      <c r="M47" s="14"/>
-      <c r="N47" s="14"/>
-      <c r="O47" s="14"/>
-      <c r="P47" s="14"/>
-      <c r="Q47" s="14"/>
-      <c r="R47" s="14"/>
-      <c r="S47" s="14"/>
       <c r="T47" s="5"/>
     </row>
     <row r="48" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B48" s="4"/>
-      <c r="C48" s="14"/>
-      <c r="D48" s="14"/>
-      <c r="E48" s="14"/>
-      <c r="F48" s="14"/>
-      <c r="G48" s="14"/>
-      <c r="H48" s="14"/>
-      <c r="I48" s="14"/>
-      <c r="J48" s="14"/>
-      <c r="K48" s="14"/>
-      <c r="L48" s="14"/>
-      <c r="M48" s="14"/>
-      <c r="N48" s="14"/>
-      <c r="O48" s="14"/>
-      <c r="P48" s="14"/>
-      <c r="Q48" s="14"/>
-      <c r="R48" s="14"/>
-      <c r="S48" s="14"/>
       <c r="T48" s="5"/>
     </row>
     <row r="49" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B49" s="4"/>
-      <c r="C49" s="14"/>
-      <c r="D49" s="14"/>
-      <c r="E49" s="14"/>
-      <c r="F49" s="14"/>
-      <c r="G49" s="14"/>
-      <c r="H49" s="14"/>
-      <c r="I49" s="14"/>
-      <c r="J49" s="14"/>
-      <c r="K49" s="14"/>
-      <c r="L49" s="14"/>
-      <c r="M49" s="14"/>
-      <c r="N49" s="14"/>
-      <c r="O49" s="14"/>
-      <c r="P49" s="14"/>
-      <c r="Q49" s="14"/>
-      <c r="R49" s="14"/>
-      <c r="S49" s="14"/>
       <c r="T49" s="5"/>
     </row>
     <row r="50" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B50" s="4"/>
-      <c r="C50" s="14"/>
-      <c r="D50" s="14"/>
-      <c r="E50" s="14"/>
-      <c r="F50" s="14"/>
-      <c r="G50" s="14"/>
-      <c r="H50" s="14"/>
-      <c r="I50" s="14"/>
-      <c r="J50" s="14"/>
-      <c r="K50" s="14"/>
-      <c r="L50" s="14"/>
-      <c r="M50" s="14"/>
-      <c r="N50" s="14"/>
-      <c r="O50" s="14"/>
-      <c r="P50" s="14"/>
-      <c r="Q50" s="14"/>
-      <c r="R50" s="14"/>
-      <c r="S50" s="14"/>
       <c r="T50" s="5"/>
     </row>
     <row r="51" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B51" s="4"/>
-      <c r="C51" s="14"/>
-      <c r="D51" s="14"/>
-      <c r="E51" s="14"/>
-      <c r="F51" s="14"/>
-      <c r="G51" s="14"/>
-      <c r="H51" s="14"/>
-      <c r="I51" s="14"/>
-      <c r="J51" s="14"/>
-      <c r="K51" s="14"/>
-      <c r="L51" s="14"/>
-      <c r="M51" s="14"/>
-      <c r="N51" s="14"/>
-      <c r="O51" s="14"/>
-      <c r="P51" s="14"/>
-      <c r="Q51" s="14"/>
-      <c r="R51" s="14"/>
-      <c r="S51" s="14"/>
       <c r="T51" s="5"/>
     </row>
     <row r="52" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B52" s="4"/>
-      <c r="C52" s="14"/>
-      <c r="D52" s="14"/>
-      <c r="E52" s="14"/>
-      <c r="F52" s="14"/>
-      <c r="G52" s="14"/>
-      <c r="H52" s="14"/>
-      <c r="I52" s="14"/>
-      <c r="J52" s="14"/>
-      <c r="K52" s="14"/>
-      <c r="L52" s="14"/>
-      <c r="M52" s="14"/>
-      <c r="N52" s="14"/>
-      <c r="O52" s="14"/>
-      <c r="P52" s="14"/>
-      <c r="Q52" s="14"/>
-      <c r="R52" s="14"/>
-      <c r="S52" s="14"/>
       <c r="T52" s="5"/>
     </row>
     <row r="53" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B53" s="4"/>
-      <c r="C53" s="14"/>
-      <c r="D53" s="14"/>
-      <c r="E53" s="14"/>
-      <c r="F53" s="14"/>
-      <c r="G53" s="14"/>
-      <c r="H53" s="14"/>
-      <c r="I53" s="14"/>
-      <c r="J53" s="14"/>
-      <c r="K53" s="14"/>
-      <c r="L53" s="14"/>
-      <c r="M53" s="14"/>
-      <c r="N53" s="14"/>
-      <c r="O53" s="14"/>
-      <c r="P53" s="14"/>
-      <c r="Q53" s="14"/>
-      <c r="R53" s="14"/>
-      <c r="S53" s="14"/>
       <c r="T53" s="5"/>
     </row>
     <row r="54" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B54" s="4"/>
-      <c r="C54" s="14"/>
-      <c r="D54" s="14"/>
-      <c r="E54" s="14"/>
-      <c r="F54" s="14"/>
-      <c r="G54" s="14"/>
-      <c r="H54" s="14"/>
-      <c r="I54" s="14"/>
-      <c r="J54" s="14"/>
-      <c r="K54" s="14"/>
-      <c r="L54" s="14"/>
-      <c r="M54" s="14"/>
-      <c r="N54" s="14"/>
-      <c r="O54" s="14"/>
-      <c r="P54" s="14"/>
-      <c r="Q54" s="14"/>
-      <c r="R54" s="14"/>
-      <c r="S54" s="14"/>
       <c r="T54" s="5"/>
     </row>
     <row r="55" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B55" s="4"/>
-      <c r="C55" s="14"/>
-      <c r="D55" s="14"/>
-      <c r="E55" s="14"/>
-      <c r="F55" s="14"/>
-      <c r="G55" s="14"/>
-      <c r="H55" s="14"/>
-      <c r="I55" s="14"/>
-      <c r="J55" s="14"/>
-      <c r="K55" s="14"/>
-      <c r="L55" s="14"/>
-      <c r="M55" s="14"/>
-      <c r="N55" s="14"/>
-      <c r="O55" s="14"/>
-      <c r="P55" s="14"/>
-      <c r="Q55" s="14"/>
-      <c r="R55" s="14"/>
-      <c r="S55" s="14"/>
       <c r="T55" s="5"/>
     </row>
     <row r="56" spans="2:20" x14ac:dyDescent="0.25">
@@ -7700,24 +7584,1064 @@
     </row>
     <row r="60" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B60" s="4"/>
-      <c r="C60" s="14"/>
-      <c r="D60" s="14"/>
-      <c r="E60" s="14"/>
-      <c r="F60" s="14"/>
-      <c r="G60" s="14"/>
-      <c r="H60" s="14"/>
-      <c r="I60" s="14"/>
-      <c r="J60" s="14"/>
-      <c r="K60" s="14"/>
-      <c r="L60" s="14"/>
-      <c r="M60" s="14"/>
-      <c r="N60" s="14"/>
-      <c r="O60" s="14"/>
-      <c r="P60" s="14"/>
-      <c r="Q60" s="14"/>
-      <c r="R60" s="14"/>
-      <c r="S60" s="14"/>
       <c r="T60" s="5"/>
+    </row>
+    <row r="61" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B61" s="4"/>
+      <c r="T61" s="5"/>
+    </row>
+    <row r="62" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B62" s="4"/>
+      <c r="T62" s="5"/>
+    </row>
+    <row r="63" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B63" s="4"/>
+      <c r="T63" s="5"/>
+    </row>
+    <row r="64" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B64" s="4"/>
+      <c r="T64" s="5"/>
+    </row>
+    <row r="65" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B65" s="4"/>
+      <c r="T65" s="5"/>
+    </row>
+    <row r="66" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B66" s="4"/>
+      <c r="T66" s="5"/>
+    </row>
+    <row r="67" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B67" s="4"/>
+      <c r="T67" s="5"/>
+    </row>
+    <row r="68" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B68" s="4"/>
+      <c r="T68" s="5"/>
+    </row>
+    <row r="69" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B69" s="4"/>
+      <c r="T69" s="5"/>
+    </row>
+    <row r="70" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B70" s="4"/>
+      <c r="T70" s="5"/>
+    </row>
+    <row r="71" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B71" s="4"/>
+      <c r="T71" s="5"/>
+    </row>
+    <row r="72" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B72" s="4"/>
+      <c r="T72" s="5"/>
+    </row>
+    <row r="73" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B73" s="4"/>
+      <c r="T73" s="5"/>
+    </row>
+    <row r="74" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B74" s="4"/>
+      <c r="T74" s="5"/>
+    </row>
+    <row r="75" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B75" s="4"/>
+      <c r="T75" s="5"/>
+    </row>
+    <row r="76" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B76" s="4"/>
+      <c r="T76" s="5"/>
+    </row>
+    <row r="77" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B77" s="4"/>
+      <c r="T77" s="5"/>
+    </row>
+    <row r="78" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B78" s="4"/>
+      <c r="T78" s="5"/>
+    </row>
+    <row r="79" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B79" s="4"/>
+      <c r="T79" s="5"/>
+    </row>
+    <row r="80" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B80" s="4"/>
+      <c r="T80" s="5"/>
+    </row>
+    <row r="81" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B81" s="4"/>
+      <c r="T81" s="5"/>
+    </row>
+    <row r="82" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B82" s="4"/>
+      <c r="T82" s="5"/>
+    </row>
+    <row r="83" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B83" s="4"/>
+      <c r="T83" s="5"/>
+    </row>
+    <row r="84" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B84" s="4"/>
+      <c r="T84" s="5"/>
+    </row>
+    <row r="85" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B85" s="4"/>
+      <c r="T85" s="5"/>
+    </row>
+    <row r="86" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B86" s="4"/>
+      <c r="T86" s="5"/>
+    </row>
+    <row r="87" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B87" s="4"/>
+      <c r="T87" s="5"/>
+    </row>
+    <row r="88" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B88" s="4"/>
+      <c r="T88" s="5"/>
+    </row>
+    <row r="89" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B89" s="4"/>
+      <c r="T89" s="5"/>
+    </row>
+    <row r="90" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B90" s="6"/>
+      <c r="C90" s="7"/>
+      <c r="D90" s="7"/>
+      <c r="E90" s="7"/>
+      <c r="F90" s="7"/>
+      <c r="G90" s="7"/>
+      <c r="H90" s="7"/>
+      <c r="I90" s="7"/>
+      <c r="J90" s="7"/>
+      <c r="K90" s="7"/>
+      <c r="L90" s="7"/>
+      <c r="M90" s="7"/>
+      <c r="N90" s="7"/>
+      <c r="O90" s="7"/>
+      <c r="P90" s="7"/>
+      <c r="Q90" s="7"/>
+      <c r="R90" s="7"/>
+      <c r="S90" s="7"/>
+      <c r="T90" s="8"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{857D5B61-53B4-4917-B6CE-D1A6918287C7}">
+  <dimension ref="A3:T90"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="K17" sqref="K17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B4" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="3"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B5" s="4"/>
+      <c r="C5" t="s">
+        <v>8</v>
+      </c>
+      <c r="H5" s="5"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B6" s="4"/>
+      <c r="C6" t="s">
+        <v>9</v>
+      </c>
+      <c r="H6" s="5"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B7" s="4"/>
+      <c r="C7" t="s">
+        <v>10</v>
+      </c>
+      <c r="H7" s="5"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B8" s="4"/>
+      <c r="C8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F8" s="11"/>
+      <c r="H8" s="5"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B9" s="4"/>
+      <c r="C9" t="s">
+        <v>12</v>
+      </c>
+      <c r="F9" s="11"/>
+      <c r="H9" s="5"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B10" s="4"/>
+      <c r="D10" t="s">
+        <v>15</v>
+      </c>
+      <c r="H10" s="5"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B11" s="4"/>
+      <c r="E11" t="s">
+        <v>16</v>
+      </c>
+      <c r="H11" s="5"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B12" s="4"/>
+      <c r="C12" s="11"/>
+      <c r="D12" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="E12" s="13"/>
+      <c r="H12" s="5"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B13" s="4"/>
+      <c r="C13" s="11"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="H13" s="5"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B14" s="4"/>
+      <c r="C14" s="11"/>
+      <c r="D14" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="E14" s="11"/>
+      <c r="H14" s="5"/>
+      <c r="I14" t="s">
+        <v>13</v>
+      </c>
+      <c r="J14" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B15" s="4"/>
+      <c r="C15" s="11"/>
+      <c r="D15" s="11"/>
+      <c r="E15" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="H15" s="5"/>
+      <c r="I15" t="s">
+        <v>13</v>
+      </c>
+      <c r="J15" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B16" s="6"/>
+      <c r="C16" s="7"/>
+      <c r="D16" s="7"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="7"/>
+      <c r="H16" s="8"/>
+    </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B20" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+      <c r="G20" s="2"/>
+      <c r="H20" s="2"/>
+      <c r="I20" s="2"/>
+      <c r="J20" s="2"/>
+      <c r="K20" s="2"/>
+      <c r="L20" s="2"/>
+      <c r="M20" s="2"/>
+      <c r="N20" s="2"/>
+      <c r="O20" s="2"/>
+      <c r="P20" s="3"/>
+    </row>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B21" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C21" s="14"/>
+      <c r="D21" s="14"/>
+      <c r="E21" s="14"/>
+      <c r="F21" s="14"/>
+      <c r="G21" s="14"/>
+      <c r="H21" s="14"/>
+      <c r="I21" s="14"/>
+      <c r="J21" s="14"/>
+      <c r="K21" s="14"/>
+      <c r="L21" s="14"/>
+      <c r="M21" s="14"/>
+      <c r="N21" s="14"/>
+      <c r="O21" s="14"/>
+      <c r="P21" s="5"/>
+      <c r="Q21" t="s">
+        <v>33</v>
+      </c>
+      <c r="R21" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B22" s="4"/>
+      <c r="C22" s="14"/>
+      <c r="D22" s="14"/>
+      <c r="E22" s="14"/>
+      <c r="F22" s="14"/>
+      <c r="G22" s="14"/>
+      <c r="H22" s="14"/>
+      <c r="I22" s="14"/>
+      <c r="J22" s="14"/>
+      <c r="K22" s="14"/>
+      <c r="L22" s="14"/>
+      <c r="M22" s="14"/>
+      <c r="N22" s="14"/>
+      <c r="O22" s="14"/>
+      <c r="P22" s="5"/>
+    </row>
+    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B23" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C23" s="14"/>
+      <c r="D23" s="14"/>
+      <c r="E23" s="14"/>
+      <c r="F23" s="14"/>
+      <c r="G23" s="14"/>
+      <c r="H23" s="14"/>
+      <c r="I23" s="14"/>
+      <c r="J23" s="14"/>
+      <c r="K23" s="14"/>
+      <c r="L23" s="14"/>
+      <c r="M23" s="14"/>
+      <c r="N23" s="14"/>
+      <c r="O23" s="14"/>
+      <c r="P23" s="5"/>
+    </row>
+    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B24" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C24" s="7"/>
+      <c r="D24" s="7"/>
+      <c r="E24" s="7"/>
+      <c r="F24" s="7"/>
+      <c r="G24" s="7"/>
+      <c r="H24" s="7"/>
+      <c r="I24" s="7"/>
+      <c r="J24" s="7"/>
+      <c r="K24" s="7"/>
+      <c r="L24" s="7"/>
+      <c r="M24" s="7"/>
+      <c r="N24" s="7"/>
+      <c r="O24" s="7"/>
+      <c r="P24" s="8"/>
+    </row>
+    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B27" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="C27" s="2"/>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2"/>
+      <c r="F27" s="2"/>
+      <c r="G27" s="2"/>
+      <c r="H27" s="2"/>
+      <c r="I27" s="2"/>
+      <c r="J27" s="2"/>
+      <c r="K27" s="2"/>
+      <c r="L27" s="2"/>
+      <c r="M27" s="2"/>
+      <c r="N27" s="2"/>
+      <c r="O27" s="2"/>
+      <c r="P27" s="2"/>
+      <c r="Q27" s="2"/>
+      <c r="R27" s="2"/>
+      <c r="S27" s="2"/>
+      <c r="T27" s="3"/>
+    </row>
+    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B28" s="4"/>
+      <c r="C28" s="14"/>
+      <c r="D28" s="14"/>
+      <c r="E28" s="14"/>
+      <c r="F28" s="14"/>
+      <c r="G28" s="14"/>
+      <c r="H28" s="14"/>
+      <c r="I28" s="14"/>
+      <c r="J28" s="14"/>
+      <c r="K28" s="14"/>
+      <c r="L28" s="14"/>
+      <c r="M28" s="14"/>
+      <c r="N28" s="14"/>
+      <c r="O28" s="14"/>
+      <c r="P28" s="14"/>
+      <c r="Q28" s="14"/>
+      <c r="R28" s="14"/>
+      <c r="S28" s="14"/>
+      <c r="T28" s="5"/>
+    </row>
+    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B29" s="4"/>
+      <c r="C29" s="14"/>
+      <c r="D29" s="14"/>
+      <c r="E29" s="14"/>
+      <c r="F29" s="14"/>
+      <c r="G29" s="14"/>
+      <c r="H29" s="14"/>
+      <c r="I29" s="14"/>
+      <c r="J29" s="14"/>
+      <c r="K29" s="14"/>
+      <c r="L29" s="14"/>
+      <c r="M29" s="14"/>
+      <c r="N29" s="14"/>
+      <c r="O29" s="14"/>
+      <c r="P29" s="14"/>
+      <c r="Q29" s="14"/>
+      <c r="R29" s="14"/>
+      <c r="S29" s="14"/>
+      <c r="T29" s="5"/>
+    </row>
+    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B30" s="4"/>
+      <c r="C30" s="14"/>
+      <c r="D30" s="14"/>
+      <c r="E30" s="14"/>
+      <c r="F30" s="14"/>
+      <c r="G30" s="14"/>
+      <c r="H30" s="14"/>
+      <c r="I30" s="14"/>
+      <c r="J30" s="14"/>
+      <c r="K30" s="14"/>
+      <c r="L30" s="14"/>
+      <c r="M30" s="14"/>
+      <c r="N30" s="14"/>
+      <c r="O30" s="14"/>
+      <c r="P30" s="14"/>
+      <c r="Q30" s="14"/>
+      <c r="R30" s="14"/>
+      <c r="S30" s="14"/>
+      <c r="T30" s="5"/>
+    </row>
+    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B31" s="4"/>
+      <c r="C31" s="14"/>
+      <c r="D31" s="14"/>
+      <c r="E31" s="14"/>
+      <c r="F31" s="14"/>
+      <c r="G31" s="14"/>
+      <c r="H31" s="14"/>
+      <c r="I31" s="14"/>
+      <c r="J31" s="14"/>
+      <c r="K31" s="14"/>
+      <c r="L31" s="14"/>
+      <c r="M31" s="14"/>
+      <c r="N31" s="14"/>
+      <c r="O31" s="14"/>
+      <c r="P31" s="14"/>
+      <c r="Q31" s="14"/>
+      <c r="R31" s="14"/>
+      <c r="S31" s="14"/>
+      <c r="T31" s="5"/>
+    </row>
+    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B32" s="4"/>
+      <c r="C32" s="14"/>
+      <c r="D32" s="14"/>
+      <c r="E32" s="14"/>
+      <c r="F32" s="14"/>
+      <c r="G32" s="14"/>
+      <c r="H32" s="14"/>
+      <c r="I32" s="14"/>
+      <c r="J32" s="14"/>
+      <c r="K32" s="14"/>
+      <c r="L32" s="14"/>
+      <c r="M32" s="14"/>
+      <c r="N32" s="14"/>
+      <c r="O32" s="14"/>
+      <c r="P32" s="14"/>
+      <c r="Q32" s="14"/>
+      <c r="R32" s="14"/>
+      <c r="S32" s="14"/>
+      <c r="T32" s="5"/>
+    </row>
+    <row r="33" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B33" s="4"/>
+      <c r="C33" s="14"/>
+      <c r="D33" s="14"/>
+      <c r="E33" s="14"/>
+      <c r="F33" s="14"/>
+      <c r="G33" s="14"/>
+      <c r="H33" s="14"/>
+      <c r="I33" s="14"/>
+      <c r="J33" s="14"/>
+      <c r="K33" s="14"/>
+      <c r="L33" s="14"/>
+      <c r="M33" s="14"/>
+      <c r="N33" s="14"/>
+      <c r="O33" s="14"/>
+      <c r="P33" s="14"/>
+      <c r="Q33" s="14"/>
+      <c r="R33" s="14"/>
+      <c r="S33" s="14"/>
+      <c r="T33" s="5"/>
+    </row>
+    <row r="34" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B34" s="4"/>
+      <c r="C34" s="14"/>
+      <c r="D34" s="14"/>
+      <c r="E34" s="14"/>
+      <c r="F34" s="14"/>
+      <c r="G34" s="14"/>
+      <c r="H34" s="14"/>
+      <c r="I34" s="14"/>
+      <c r="J34" s="14"/>
+      <c r="K34" s="14"/>
+      <c r="L34" s="14"/>
+      <c r="M34" s="14"/>
+      <c r="N34" s="14"/>
+      <c r="O34" s="14"/>
+      <c r="P34" s="14"/>
+      <c r="Q34" s="14"/>
+      <c r="R34" s="14"/>
+      <c r="S34" s="14"/>
+      <c r="T34" s="5"/>
+    </row>
+    <row r="35" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B35" s="4"/>
+      <c r="C35" s="14"/>
+      <c r="D35" s="14"/>
+      <c r="E35" s="14"/>
+      <c r="F35" s="14"/>
+      <c r="G35" s="14"/>
+      <c r="H35" s="14"/>
+      <c r="I35" s="14"/>
+      <c r="J35" s="14"/>
+      <c r="K35" s="14"/>
+      <c r="L35" s="14"/>
+      <c r="M35" s="14"/>
+      <c r="N35" s="14"/>
+      <c r="O35" s="14"/>
+      <c r="P35" s="14"/>
+      <c r="Q35" s="14"/>
+      <c r="R35" s="14"/>
+      <c r="S35" s="14"/>
+      <c r="T35" s="5"/>
+    </row>
+    <row r="36" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B36" s="4"/>
+      <c r="C36" s="14"/>
+      <c r="D36" s="14"/>
+      <c r="E36" s="14"/>
+      <c r="F36" s="14"/>
+      <c r="G36" s="14"/>
+      <c r="H36" s="14"/>
+      <c r="I36" s="14"/>
+      <c r="J36" s="14"/>
+      <c r="K36" s="14"/>
+      <c r="L36" s="14"/>
+      <c r="M36" s="14"/>
+      <c r="N36" s="14"/>
+      <c r="O36" s="14"/>
+      <c r="P36" s="14"/>
+      <c r="Q36" s="14"/>
+      <c r="R36" s="14"/>
+      <c r="S36" s="14"/>
+      <c r="T36" s="5"/>
+    </row>
+    <row r="37" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B37" s="4"/>
+      <c r="C37" s="14"/>
+      <c r="D37" s="14"/>
+      <c r="E37" s="14"/>
+      <c r="F37" s="14"/>
+      <c r="G37" s="14"/>
+      <c r="H37" s="14"/>
+      <c r="I37" s="14"/>
+      <c r="J37" s="14"/>
+      <c r="K37" s="14"/>
+      <c r="L37" s="14"/>
+      <c r="M37" s="14"/>
+      <c r="N37" s="14"/>
+      <c r="O37" s="14"/>
+      <c r="P37" s="14"/>
+      <c r="Q37" s="14"/>
+      <c r="R37" s="14"/>
+      <c r="S37" s="14"/>
+      <c r="T37" s="5"/>
+    </row>
+    <row r="38" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B38" s="4"/>
+      <c r="C38" s="14"/>
+      <c r="D38" s="14"/>
+      <c r="E38" s="14"/>
+      <c r="F38" s="14"/>
+      <c r="G38" s="14"/>
+      <c r="H38" s="14"/>
+      <c r="I38" s="14"/>
+      <c r="J38" s="14"/>
+      <c r="K38" s="14"/>
+      <c r="L38" s="14"/>
+      <c r="M38" s="14"/>
+      <c r="N38" s="14"/>
+      <c r="O38" s="14"/>
+      <c r="P38" s="14"/>
+      <c r="Q38" s="14"/>
+      <c r="R38" s="14"/>
+      <c r="S38" s="14"/>
+      <c r="T38" s="5"/>
+    </row>
+    <row r="39" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B39" s="4"/>
+      <c r="C39" s="14"/>
+      <c r="D39" s="14"/>
+      <c r="E39" s="14"/>
+      <c r="F39" s="14"/>
+      <c r="G39" s="14"/>
+      <c r="H39" s="14"/>
+      <c r="I39" s="14"/>
+      <c r="J39" s="14"/>
+      <c r="K39" s="14"/>
+      <c r="L39" s="14"/>
+      <c r="M39" s="14"/>
+      <c r="N39" s="14"/>
+      <c r="O39" s="14"/>
+      <c r="P39" s="14"/>
+      <c r="Q39" s="14"/>
+      <c r="R39" s="14"/>
+      <c r="S39" s="14"/>
+      <c r="T39" s="5"/>
+    </row>
+    <row r="40" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B40" s="4"/>
+      <c r="C40" s="14"/>
+      <c r="D40" s="14"/>
+      <c r="E40" s="14"/>
+      <c r="F40" s="14"/>
+      <c r="G40" s="14"/>
+      <c r="H40" s="14"/>
+      <c r="I40" s="14"/>
+      <c r="J40" s="14"/>
+      <c r="K40" s="14"/>
+      <c r="L40" s="14"/>
+      <c r="M40" s="14"/>
+      <c r="N40" s="14"/>
+      <c r="O40" s="14"/>
+      <c r="P40" s="14"/>
+      <c r="Q40" s="14"/>
+      <c r="R40" s="14"/>
+      <c r="S40" s="14"/>
+      <c r="T40" s="5"/>
+    </row>
+    <row r="41" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B41" s="4"/>
+      <c r="C41" s="14"/>
+      <c r="D41" s="14"/>
+      <c r="E41" s="14"/>
+      <c r="F41" s="14"/>
+      <c r="G41" s="14"/>
+      <c r="H41" s="14"/>
+      <c r="I41" s="14"/>
+      <c r="J41" s="14"/>
+      <c r="K41" s="14"/>
+      <c r="L41" s="14"/>
+      <c r="M41" s="14"/>
+      <c r="N41" s="14"/>
+      <c r="O41" s="14"/>
+      <c r="P41" s="14"/>
+      <c r="Q41" s="14"/>
+      <c r="R41" s="14"/>
+      <c r="S41" s="14"/>
+      <c r="T41" s="5"/>
+    </row>
+    <row r="42" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B42" s="4"/>
+      <c r="C42" s="14"/>
+      <c r="D42" s="14"/>
+      <c r="E42" s="14"/>
+      <c r="F42" s="14"/>
+      <c r="G42" s="14"/>
+      <c r="H42" s="14"/>
+      <c r="I42" s="14"/>
+      <c r="J42" s="14"/>
+      <c r="K42" s="14"/>
+      <c r="L42" s="14"/>
+      <c r="M42" s="14"/>
+      <c r="N42" s="14"/>
+      <c r="O42" s="14"/>
+      <c r="P42" s="14"/>
+      <c r="Q42" s="14"/>
+      <c r="R42" s="14"/>
+      <c r="S42" s="14"/>
+      <c r="T42" s="5"/>
+    </row>
+    <row r="43" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B43" s="4"/>
+      <c r="C43" s="14"/>
+      <c r="D43" s="14"/>
+      <c r="E43" s="14"/>
+      <c r="F43" s="14"/>
+      <c r="G43" s="14"/>
+      <c r="H43" s="14"/>
+      <c r="I43" s="14"/>
+      <c r="J43" s="14"/>
+      <c r="K43" s="14"/>
+      <c r="L43" s="14"/>
+      <c r="M43" s="14"/>
+      <c r="N43" s="14"/>
+      <c r="O43" s="14"/>
+      <c r="P43" s="14"/>
+      <c r="Q43" s="14"/>
+      <c r="R43" s="14"/>
+      <c r="S43" s="14"/>
+      <c r="T43" s="5"/>
+    </row>
+    <row r="44" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B44" s="4"/>
+      <c r="C44" s="14"/>
+      <c r="D44" s="14"/>
+      <c r="E44" s="14"/>
+      <c r="F44" s="14"/>
+      <c r="G44" s="14"/>
+      <c r="H44" s="14"/>
+      <c r="I44" s="14"/>
+      <c r="J44" s="14"/>
+      <c r="K44" s="14"/>
+      <c r="L44" s="14"/>
+      <c r="M44" s="14"/>
+      <c r="N44" s="14"/>
+      <c r="O44" s="14"/>
+      <c r="P44" s="14"/>
+      <c r="Q44" s="14"/>
+      <c r="R44" s="14"/>
+      <c r="S44" s="14"/>
+      <c r="T44" s="5"/>
+    </row>
+    <row r="45" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B45" s="4"/>
+      <c r="C45" s="14"/>
+      <c r="D45" s="14"/>
+      <c r="E45" s="14"/>
+      <c r="F45" s="14"/>
+      <c r="G45" s="14"/>
+      <c r="H45" s="14"/>
+      <c r="I45" s="14"/>
+      <c r="J45" s="14"/>
+      <c r="K45" s="14"/>
+      <c r="L45" s="14"/>
+      <c r="M45" s="14"/>
+      <c r="N45" s="14"/>
+      <c r="O45" s="14"/>
+      <c r="P45" s="14"/>
+      <c r="Q45" s="14"/>
+      <c r="R45" s="14"/>
+      <c r="S45" s="14"/>
+      <c r="T45" s="5"/>
+    </row>
+    <row r="46" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B46" s="4"/>
+      <c r="C46" s="14"/>
+      <c r="D46" s="14"/>
+      <c r="E46" s="14"/>
+      <c r="F46" s="14"/>
+      <c r="G46" s="14"/>
+      <c r="H46" s="14"/>
+      <c r="I46" s="14"/>
+      <c r="J46" s="14"/>
+      <c r="K46" s="14"/>
+      <c r="L46" s="14"/>
+      <c r="M46" s="14"/>
+      <c r="N46" s="14"/>
+      <c r="O46" s="14"/>
+      <c r="P46" s="14"/>
+      <c r="Q46" s="14"/>
+      <c r="R46" s="14"/>
+      <c r="S46" s="14"/>
+      <c r="T46" s="5"/>
+    </row>
+    <row r="47" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B47" s="4"/>
+      <c r="C47" s="14"/>
+      <c r="D47" s="14"/>
+      <c r="E47" s="14"/>
+      <c r="F47" s="14"/>
+      <c r="G47" s="14"/>
+      <c r="H47" s="14"/>
+      <c r="I47" s="14"/>
+      <c r="J47" s="14"/>
+      <c r="K47" s="14"/>
+      <c r="L47" s="14"/>
+      <c r="M47" s="14"/>
+      <c r="N47" s="14"/>
+      <c r="O47" s="14"/>
+      <c r="P47" s="14"/>
+      <c r="Q47" s="14"/>
+      <c r="R47" s="14"/>
+      <c r="S47" s="14"/>
+      <c r="T47" s="5"/>
+    </row>
+    <row r="48" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B48" s="4"/>
+      <c r="C48" s="14"/>
+      <c r="D48" s="14"/>
+      <c r="E48" s="14"/>
+      <c r="F48" s="14"/>
+      <c r="G48" s="14"/>
+      <c r="H48" s="14"/>
+      <c r="I48" s="14"/>
+      <c r="J48" s="14"/>
+      <c r="K48" s="14"/>
+      <c r="L48" s="14"/>
+      <c r="M48" s="14"/>
+      <c r="N48" s="14"/>
+      <c r="O48" s="14"/>
+      <c r="P48" s="14"/>
+      <c r="Q48" s="14"/>
+      <c r="R48" s="14"/>
+      <c r="S48" s="14"/>
+      <c r="T48" s="5"/>
+    </row>
+    <row r="49" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B49" s="4"/>
+      <c r="C49" s="14"/>
+      <c r="D49" s="14"/>
+      <c r="E49" s="14"/>
+      <c r="F49" s="14"/>
+      <c r="G49" s="14"/>
+      <c r="H49" s="14"/>
+      <c r="I49" s="14"/>
+      <c r="J49" s="14"/>
+      <c r="K49" s="14"/>
+      <c r="L49" s="14"/>
+      <c r="M49" s="14"/>
+      <c r="N49" s="14"/>
+      <c r="O49" s="14"/>
+      <c r="P49" s="14"/>
+      <c r="Q49" s="14"/>
+      <c r="R49" s="14"/>
+      <c r="S49" s="14"/>
+      <c r="T49" s="5"/>
+    </row>
+    <row r="50" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B50" s="4"/>
+      <c r="C50" s="14"/>
+      <c r="D50" s="14"/>
+      <c r="E50" s="14"/>
+      <c r="F50" s="14"/>
+      <c r="G50" s="14"/>
+      <c r="H50" s="14"/>
+      <c r="I50" s="14"/>
+      <c r="J50" s="14"/>
+      <c r="K50" s="14"/>
+      <c r="L50" s="14"/>
+      <c r="M50" s="14"/>
+      <c r="N50" s="14"/>
+      <c r="O50" s="14"/>
+      <c r="P50" s="14"/>
+      <c r="Q50" s="14"/>
+      <c r="R50" s="14"/>
+      <c r="S50" s="14"/>
+      <c r="T50" s="5"/>
+    </row>
+    <row r="51" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B51" s="4"/>
+      <c r="C51" s="14"/>
+      <c r="D51" s="14"/>
+      <c r="E51" s="14"/>
+      <c r="F51" s="14"/>
+      <c r="G51" s="14"/>
+      <c r="H51" s="14"/>
+      <c r="I51" s="14"/>
+      <c r="J51" s="14"/>
+      <c r="K51" s="14"/>
+      <c r="L51" s="14"/>
+      <c r="M51" s="14"/>
+      <c r="N51" s="14"/>
+      <c r="O51" s="14"/>
+      <c r="P51" s="14"/>
+      <c r="Q51" s="14"/>
+      <c r="R51" s="14"/>
+      <c r="S51" s="14"/>
+      <c r="T51" s="5"/>
+    </row>
+    <row r="52" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B52" s="4"/>
+      <c r="C52" s="14"/>
+      <c r="D52" s="14"/>
+      <c r="E52" s="14"/>
+      <c r="F52" s="14"/>
+      <c r="G52" s="14"/>
+      <c r="H52" s="14"/>
+      <c r="I52" s="14"/>
+      <c r="J52" s="14"/>
+      <c r="K52" s="14"/>
+      <c r="L52" s="14"/>
+      <c r="M52" s="14"/>
+      <c r="N52" s="14"/>
+      <c r="O52" s="14"/>
+      <c r="P52" s="14"/>
+      <c r="Q52" s="14"/>
+      <c r="R52" s="14"/>
+      <c r="S52" s="14"/>
+      <c r="T52" s="5"/>
+    </row>
+    <row r="53" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B53" s="4"/>
+      <c r="C53" s="14"/>
+      <c r="D53" s="14"/>
+      <c r="E53" s="14"/>
+      <c r="F53" s="14"/>
+      <c r="G53" s="14"/>
+      <c r="H53" s="14"/>
+      <c r="I53" s="14"/>
+      <c r="J53" s="14"/>
+      <c r="K53" s="14"/>
+      <c r="L53" s="14"/>
+      <c r="M53" s="14"/>
+      <c r="N53" s="14"/>
+      <c r="O53" s="14"/>
+      <c r="P53" s="14"/>
+      <c r="Q53" s="14"/>
+      <c r="R53" s="14"/>
+      <c r="S53" s="14"/>
+      <c r="T53" s="5"/>
+    </row>
+    <row r="54" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B54" s="4"/>
+      <c r="C54" s="14"/>
+      <c r="D54" s="14"/>
+      <c r="E54" s="14"/>
+      <c r="F54" s="14"/>
+      <c r="G54" s="14"/>
+      <c r="H54" s="14"/>
+      <c r="I54" s="14"/>
+      <c r="J54" s="14"/>
+      <c r="K54" s="14"/>
+      <c r="L54" s="14"/>
+      <c r="M54" s="14"/>
+      <c r="N54" s="14"/>
+      <c r="O54" s="14"/>
+      <c r="P54" s="14"/>
+      <c r="Q54" s="14"/>
+      <c r="R54" s="14"/>
+      <c r="S54" s="14"/>
+      <c r="T54" s="5"/>
+    </row>
+    <row r="55" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B55" s="4"/>
+      <c r="C55" s="14"/>
+      <c r="D55" s="14"/>
+      <c r="E55" s="14"/>
+      <c r="F55" s="14"/>
+      <c r="G55" s="14"/>
+      <c r="H55" s="14"/>
+      <c r="I55" s="14"/>
+      <c r="J55" s="14"/>
+      <c r="K55" s="14"/>
+      <c r="L55" s="14"/>
+      <c r="M55" s="14"/>
+      <c r="N55" s="14"/>
+      <c r="O55" s="14"/>
+      <c r="P55" s="14"/>
+      <c r="Q55" s="14"/>
+      <c r="R55" s="14"/>
+      <c r="S55" s="14"/>
+      <c r="T55" s="5"/>
+    </row>
+    <row r="56" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B56" s="4"/>
+      <c r="C56" s="14"/>
+      <c r="D56" s="14"/>
+      <c r="E56" s="14"/>
+      <c r="F56" s="14"/>
+      <c r="G56" s="14"/>
+      <c r="H56" s="14"/>
+      <c r="I56" s="14"/>
+      <c r="J56" s="14"/>
+      <c r="K56" s="14"/>
+      <c r="L56" s="14"/>
+      <c r="M56" s="14"/>
+      <c r="N56" s="14"/>
+      <c r="O56" s="14"/>
+      <c r="P56" s="14"/>
+      <c r="Q56" s="14"/>
+      <c r="R56" s="14"/>
+      <c r="S56" s="14"/>
+      <c r="T56" s="5"/>
+    </row>
+    <row r="57" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B57" s="6"/>
+      <c r="C57" s="7"/>
+      <c r="D57" s="7"/>
+      <c r="E57" s="7"/>
+      <c r="F57" s="7"/>
+      <c r="G57" s="7"/>
+      <c r="H57" s="7"/>
+      <c r="I57" s="7"/>
+      <c r="J57" s="7"/>
+      <c r="K57" s="7"/>
+      <c r="L57" s="7"/>
+      <c r="M57" s="7"/>
+      <c r="N57" s="7"/>
+      <c r="O57" s="7"/>
+      <c r="P57" s="7"/>
+      <c r="Q57" s="7"/>
+      <c r="R57" s="7"/>
+      <c r="S57" s="7"/>
+      <c r="T57" s="8"/>
+    </row>
+    <row r="60" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B60" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="C60" s="2"/>
+      <c r="D60" s="2"/>
+      <c r="E60" s="2"/>
+      <c r="F60" s="2"/>
+      <c r="G60" s="2"/>
+      <c r="H60" s="2"/>
+      <c r="I60" s="2"/>
+      <c r="J60" s="2"/>
+      <c r="K60" s="2"/>
+      <c r="L60" s="2"/>
+      <c r="M60" s="2"/>
+      <c r="N60" s="2"/>
+      <c r="O60" s="2"/>
+      <c r="P60" s="2"/>
+      <c r="Q60" s="2"/>
+      <c r="R60" s="2"/>
+      <c r="S60" s="2"/>
+      <c r="T60" s="3"/>
     </row>
     <row r="61" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B61" s="4"/>

</xml_diff>